<commit_message>
MainBoard: - change pinout of ESP and STM - change pinout of UIboard connector - add support for ESP debugging over JTAG through STM - add USB cable insertion detection - add 1k5 pull resistor to USB D+ - add USB_C - add MPU-6050 - add step-down for intelligent leds - add ESP reset button - add test points - replace expander connector by pinheads - connect I2C display - connect intelligent servos to STM, instead of ESP - fix AMS1117 4th pin connection - move some connectors - renumber schematic - reorder sheets
</commit_message>
<xml_diff>
--- a/ele/MainBoard/parts.xlsx
+++ b/ele/MainBoard/parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\working\RB3204-RBCX\ele\MainBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{99CD2A55-9FD2-4E23-8ECE-501E5F0B2B33}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{9FC7F01E-88C6-42AD-9A9C-627D40291EB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JLC" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <customWorkbookView name="kubas – osobní zobrazení" guid="{ECED9359-1734-47D7-B3C3-7708E1EFED96}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1066" activeSheetId="1"/>
     <customWorkbookView name="Jaroslav PARAL - Personal View" guid="{021D7215-5824-4286-91FC-F56FA6AECCD0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1416" activeSheetId="1"/>
   </customWorkbookViews>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -110,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="357">
   <si>
     <t>ID</t>
   </si>
@@ -1166,6 +1167,21 @@
   </si>
   <si>
     <t>https://www.aliexpress.com/item/33042530151.html?spm=a2g0o.detail.1000060.3.413116e3UwnGSp&amp;gps-id=pcDetailBottomMoreThisSeller&amp;scm=1007.14977.161855.0&amp;scm_id=1007.14977.161855.0&amp;scm-url=1007.14977.161855.0&amp;pvid=e7acc9bf-7b2c-452a-9ec7-bda6f01c289c&amp;_t=gps-id:pcDetailBottomMoreThisSeller,scm-url:1007.14977.161855.0,pvid:e7acc9bf-7b2c-452a-9ec7-bda6f01c289c,tpp_buckets:668%230%23165478%2314_668%23808%234093%23880_668%23888%233325%234</t>
+  </si>
+  <si>
+    <t>R118</t>
+  </si>
+  <si>
+    <t>1k5</t>
+  </si>
+  <si>
+    <t>R0403</t>
+  </si>
+  <si>
+    <t>C25867</t>
+  </si>
+  <si>
+    <t>0402WGF1501TCE</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1192,7 @@
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.0000"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1219,6 +1235,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1290,7 +1313,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0FA74BC0-0743-490A-98AF-D5A1678D9E55}" diskRevisions="1" revisionId="89" version="5">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{E20A599C-5D52-40E3-BA19-8EED18B308A9}" diskRevisions="1" revisionId="105" version="6">
   <header guid="{08FCBB00-DC5A-40BD-80BF-EC6CE43DA19E}" dateTime="2020-03-28T18:14:29" maxSheetId="5" userName="Jaroslav PARAL" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -1334,6 +1357,14 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{E20A599C-5D52-40E3-BA19-8EED18B308A9}" dateTime="2020-04-21T12:19:19" maxSheetId="5" userName="kubas" r:id="rId6" minRId="90" maxRId="105">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -1991,9 +2022,108 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="90" sId="1" ref="A30:XFD30" action="insertRow"/>
+  <rcc rId="91" sId="1">
+    <nc r="A30">
+      <v>1</v>
+    </nc>
+  </rcc>
+  <rcc rId="92" sId="1">
+    <nc r="B30" t="inlineStr">
+      <is>
+        <t>R118</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="93" sId="1">
+    <nc r="C30" t="inlineStr">
+      <is>
+        <t>1k5</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="94" sId="1">
+    <nc r="E30" t="inlineStr">
+      <is>
+        <t>Uniroyal Elec</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="95" sId="1">
+    <nc r="G30" t="inlineStr">
+      <is>
+        <t>R0403</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="96" sId="1">
+    <nc r="I30" t="inlineStr">
+      <is>
+        <t>NO</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="97" sId="1" numFmtId="11">
+    <nc r="J30">
+      <v>8.9999999999999998E-4</v>
+    </nc>
+  </rcc>
+  <rcc rId="98" sId="1" numFmtId="11">
+    <nc r="Q30">
+      <v>2.9999999999999997E-4</v>
+    </nc>
+  </rcc>
+  <rcc rId="99" sId="1">
+    <nc r="T30">
+      <f>A30*J30+ (A30*H30*0.0015)</f>
+    </nc>
+  </rcc>
+  <rcc rId="100" sId="1">
+    <nc r="U30">
+      <f>A30*50</f>
+    </nc>
+  </rcc>
+  <rcc rId="101" sId="1">
+    <nc r="Y30" t="inlineStr">
+      <is>
+        <t>CHIP RESISTOR ±1% 1/16W</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="102" sId="1" numFmtId="19">
+    <nc r="S30">
+      <v>43941</v>
+    </nc>
+  </rcc>
+  <rcc rId="103" sId="1">
+    <nc r="H30">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="104" sId="1">
+    <nc r="F30" t="inlineStr">
+      <is>
+        <t>C25867</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="105" sId="1" xfDxf="1" dxf="1">
+    <nc r="D30" t="inlineStr">
+      <is>
+        <t>0402WGF1501TCE</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="3">
   <userInfo guid="{66346596-386A-4DB2-A9FA-EF15037E4AF8}" name="kubas" id="-1003731210" dateTime="2020-04-06T17:53:41"/>
+  <userInfo guid="{0FA74BC0-0743-490A-98AF-D5A1678D9E55}" name="kubas" id="-1003696187" dateTime="2020-04-20T18:20:21"/>
+  <userInfo guid="{E20A599C-5D52-40E3-BA19-8EED18B308A9}" name="kubas" id="-1003713540" dateTime="2020-04-21T11:54:59"/>
 </users>
 </file>
 
@@ -2294,7 +2424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y40"/>
+  <dimension ref="A1:Y41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2458,7 +2588,7 @@
         <v>43917</v>
       </c>
       <c r="T2" s="9">
-        <f t="shared" ref="T2:T36" si="0">A2*J2+ (A2*H2*0.0015)</f>
+        <f t="shared" ref="T2:T37" si="0">A2*J2+ (A2*H2*0.0015)</f>
         <v>2.5787</v>
       </c>
       <c r="U2" s="11">
@@ -2533,7 +2663,7 @@
         <v>3.2143999999999999</v>
       </c>
       <c r="U3" s="11">
-        <f t="shared" ref="U3:U36" si="1">A3*50</f>
+        <f t="shared" ref="U3:U37" si="1">A3*50</f>
         <v>400</v>
       </c>
       <c r="V3" s="9"/>
@@ -4110,25 +4240,25 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>297</v>
+        <v>352</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>353</v>
       </c>
       <c r="D30" t="s">
-        <v>267</v>
+        <v>356</v>
       </c>
       <c r="E30" t="s">
         <v>256</v>
       </c>
       <c r="F30" t="s">
-        <v>268</v>
+        <v>355</v>
       </c>
       <c r="G30" t="s">
-        <v>30</v>
+        <v>354</v>
       </c>
       <c r="H30">
         <v>2</v>
@@ -4150,15 +4280,15 @@
       </c>
       <c r="R30" s="5"/>
       <c r="S30" s="2">
-        <v>43917</v>
+        <v>43941</v>
       </c>
       <c r="T30" s="9">
-        <f t="shared" si="0"/>
-        <v>5.4600000000000003E-2</v>
+        <f t="shared" ref="T30" si="2">A30*J30+ (A30*H30*0.0015)</f>
+        <v>3.8999999999999998E-3</v>
       </c>
       <c r="U30" s="11">
-        <f t="shared" si="1"/>
-        <v>700</v>
+        <f t="shared" ref="U30" si="3">A30*50</f>
+        <v>50</v>
       </c>
       <c r="V30" s="9"/>
       <c r="X30" s="7"/>
@@ -4168,22 +4298,22 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D31" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E31" t="s">
         <v>256</v>
       </c>
       <c r="F31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G31" t="s">
         <v>30</v>
@@ -4212,11 +4342,11 @@
       </c>
       <c r="T31" s="9">
         <f t="shared" si="0"/>
-        <v>4.2900000000000001E-2</v>
+        <v>5.4600000000000003E-2</v>
       </c>
       <c r="U31" s="11">
         <f t="shared" si="1"/>
-        <v>550</v>
+        <v>700</v>
       </c>
       <c r="V31" s="9"/>
       <c r="X31" s="7"/>
@@ -4226,22 +4356,22 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E32" t="s">
         <v>256</v>
       </c>
       <c r="F32" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G32" t="s">
         <v>30</v>
@@ -4253,7 +4383,7 @@
         <v>39</v>
       </c>
       <c r="J32" s="5">
-        <v>1.1000000000000001E-3</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
@@ -4262,7 +4392,7 @@
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
       <c r="Q32" s="5">
-        <v>4.0000000000000002E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="R32" s="5"/>
       <c r="S32" s="2">
@@ -4270,11 +4400,11 @@
       </c>
       <c r="T32" s="9">
         <f t="shared" si="0"/>
-        <v>4.1000000000000003E-3</v>
+        <v>4.2900000000000001E-2</v>
       </c>
       <c r="U32" s="11">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>550</v>
       </c>
       <c r="V32" s="9"/>
       <c r="X32" s="7"/>
@@ -4284,22 +4414,22 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="D33" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E33" t="s">
         <v>256</v>
       </c>
       <c r="F33" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G33" t="s">
         <v>30</v>
@@ -4311,7 +4441,7 @@
         <v>39</v>
       </c>
       <c r="J33" s="5">
-        <v>8.9999999999999998E-4</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
@@ -4320,7 +4450,7 @@
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="5">
-        <v>2.9999999999999997E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="R33" s="5"/>
       <c r="S33" s="2">
@@ -4328,11 +4458,11 @@
       </c>
       <c r="T33" s="9">
         <f t="shared" si="0"/>
-        <v>2.3400000000000004E-2</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="U33" s="11">
         <f t="shared" si="1"/>
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="V33" s="9"/>
       <c r="X33" s="7"/>
@@ -4342,22 +4472,22 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E34" t="s">
         <v>256</v>
       </c>
       <c r="F34" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G34" t="s">
         <v>30</v>
@@ -4369,7 +4499,7 @@
         <v>39</v>
       </c>
       <c r="J34" s="5">
-        <v>1.1000000000000001E-3</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
@@ -4378,7 +4508,7 @@
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
       <c r="Q34" s="5">
-        <v>4.0000000000000002E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="R34" s="5"/>
       <c r="S34" s="2">
@@ -4386,11 +4516,11 @@
       </c>
       <c r="T34" s="9">
         <f t="shared" si="0"/>
-        <v>4.1000000000000003E-3</v>
+        <v>2.3400000000000004E-2</v>
       </c>
       <c r="U34" s="11">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="V34" s="9"/>
       <c r="X34" s="7"/>
@@ -4400,22 +4530,22 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C35" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D35" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E35" t="s">
         <v>256</v>
       </c>
       <c r="F35" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G35" t="s">
         <v>30</v>
@@ -4427,7 +4557,7 @@
         <v>39</v>
       </c>
       <c r="J35" s="5">
-        <v>1.9E-3</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
@@ -4436,7 +4566,7 @@
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
       <c r="Q35" s="5">
-        <v>5.9999999999999995E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="R35" s="5"/>
       <c r="S35" s="2">
@@ -4444,11 +4574,11 @@
       </c>
       <c r="T35" s="9">
         <f t="shared" si="0"/>
-        <v>3.4299999999999997E-2</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="U35" s="11">
         <f t="shared" si="1"/>
-        <v>350</v>
+        <v>50</v>
       </c>
       <c r="V35" s="9"/>
       <c r="X35" s="7"/>
@@ -4458,22 +4588,22 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C36" t="s">
-        <v>280</v>
+        <v>29</v>
       </c>
       <c r="D36" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E36" t="s">
         <v>256</v>
       </c>
       <c r="F36" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G36" t="s">
         <v>30</v>
@@ -4485,7 +4615,7 @@
         <v>39</v>
       </c>
       <c r="J36" s="5">
-        <v>8.9999999999999998E-4</v>
+        <v>1.9E-3</v>
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
@@ -4494,7 +4624,7 @@
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
       <c r="Q36" s="5">
-        <v>2.9999999999999997E-4</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="R36" s="5"/>
       <c r="S36" s="2">
@@ -4502,11 +4632,11 @@
       </c>
       <c r="T36" s="9">
         <f t="shared" si="0"/>
-        <v>7.7999999999999996E-3</v>
+        <v>3.4299999999999997E-2</v>
       </c>
       <c r="U36" s="11">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="V36" s="9"/>
       <c r="X36" s="7"/>
@@ -4515,33 +4645,91 @@
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="I37">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>303</v>
+      </c>
+      <c r="C37" t="s">
+        <v>280</v>
+      </c>
+      <c r="D37" t="s">
+        <v>279</v>
+      </c>
+      <c r="E37" t="s">
+        <v>256</v>
+      </c>
+      <c r="F37" t="s">
+        <v>281</v>
+      </c>
+      <c r="G37" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J37" s="5">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="R37" s="5"/>
+      <c r="S37" s="2">
+        <v>43917</v>
+      </c>
+      <c r="T37" s="9">
+        <f t="shared" si="0"/>
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="U37" s="11">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="V37" s="9"/>
+      <c r="X37" s="7"/>
+      <c r="Y37" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I38">
         <v>7</v>
       </c>
-      <c r="T37" s="9">
-        <f>SUM(T2:T36)</f>
-        <v>11.0793</v>
-      </c>
-      <c r="V37" s="9"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="H38" s="9">
+      <c r="T38" s="9">
+        <f>SUM(T2:T37)</f>
+        <v>11.0832</v>
+      </c>
+      <c r="V38" s="9"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H39" s="9">
         <v>7</v>
       </c>
-      <c r="I38" s="9">
-        <f>3*I37</f>
+      <c r="I39" s="9">
+        <f>3*I38</f>
         <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="I39" s="9">
-        <f>SUM(H38:I38)</f>
-        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="I40" s="9">
-        <f>I39/50</f>
+        <f>SUM(H39:I39)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I41" s="9">
+        <f>I40/50</f>
         <v>0.56000000000000005</v>
       </c>
     </row>
@@ -4558,6 +4746,7 @@
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
     </customSheetView>
   </customSheetViews>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>

</xml_diff>

<commit_message>
MainBoardBRD: routing (backup before processor move)
</commit_message>
<xml_diff>
--- a/ele/MainBoard/parts.xlsx
+++ b/ele/MainBoard/parts.xlsx
@@ -1314,33 +1314,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{E20A599C-5D52-40E3-BA19-8EED18B308A9}" diskRevisions="1" revisionId="105" version="6">
-  <header guid="{08FCBB00-DC5A-40BD-80BF-EC6CE43DA19E}" dateTime="2020-03-28T18:14:29" maxSheetId="5" userName="Jaroslav PARAL" r:id="rId1">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{1748B5B3-A782-4C1C-9621-94605AD6F297}" dateTime="2020-03-28T18:14:53" maxSheetId="5" userName="Jaroslav PARAL" r:id="rId2" minRId="1">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{FD5D90DF-6B85-4BA1-BBFC-34AFB2C32459}" dateTime="2020-03-29T21:24:46" maxSheetId="5" userName="Jaroslav PARAL" r:id="rId3" minRId="2" maxRId="81">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-    <reviewedList count="1">
-      <reviewed rId="2"/>
-    </reviewedList>
-  </header>
   <header guid="{66346596-386A-4DB2-A9FA-EF15037E4AF8}" dateTime="2020-03-29T21:48:07" maxSheetId="5" userName="Jaroslav PARAL" r:id="rId4" minRId="82" maxRId="89">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -1366,593 +1339,6 @@
     </sheetIdMap>
   </header>
 </headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1" sId="1" numFmtId="11">
-    <nc r="P15">
-      <v>43</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="2" ua="1" sId="1">
-    <nc r="P15"/>
-  </rcc>
-  <rcft rId="1" ua="1" sheetId="1"/>
-  <rcc rId="3" sId="1">
-    <oc r="H4">
-      <v>17</v>
-    </oc>
-    <nc r="H4">
-      <v>16</v>
-    </nc>
-  </rcc>
-  <rcc rId="4" sId="1" numFmtId="11">
-    <oc r="K5">
-      <v>0.123</v>
-    </oc>
-    <nc r="K5"/>
-  </rcc>
-  <rcc rId="5" sId="1" numFmtId="11">
-    <nc r="R6">
-      <v>0.1203</v>
-    </nc>
-  </rcc>
-  <rcc rId="6" sId="1" numFmtId="11">
-    <oc r="J7">
-      <v>2.3599999999999999E-2</v>
-    </oc>
-    <nc r="J7">
-      <v>2.18E-2</v>
-    </nc>
-  </rcc>
-  <rcc rId="7" sId="1" numFmtId="11">
-    <oc r="O7">
-      <v>1.1299999999999999E-2</v>
-    </oc>
-    <nc r="O7">
-      <v>1.04E-2</v>
-    </nc>
-  </rcc>
-  <rcc rId="8" sId="1" numFmtId="19">
-    <oc r="S7">
-      <v>43915</v>
-    </oc>
-    <nc r="S7">
-      <v>43918</v>
-    </nc>
-  </rcc>
-  <rcc rId="9" sId="1" xfDxf="1" dxf="1">
-    <oc r="F8" t="inlineStr">
-      <is>
-        <t>C305445</t>
-      </is>
-    </oc>
-    <nc r="F8" t="inlineStr">
-      <is>
-        <t>C8598</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="10" sId="1">
-    <oc r="W11" t="inlineStr">
-      <is>
-        <t>40V 3A 550mV @ 3A DO-214AC Schottky Barrier Diodes (SBD) RoHS</t>
-      </is>
-    </oc>
-    <nc r="W11" t="inlineStr">
-      <is>
-        <t>40V 3A 400mV @ 1A 550mV @ 3A DO-214AC Schottky Barrier Diodes (SBD) RoHS</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="11" sId="1">
-    <oc r="C17" t="inlineStr">
-      <is>
-        <t>32kHz</t>
-      </is>
-    </oc>
-    <nc r="C17" t="inlineStr">
-      <is>
-        <t>32.768Hz</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="12" sId="1">
-    <oc r="W29" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR</t>
-      </is>
-    </oc>
-    <nc r="W29" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR ±1% 1/16W</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="13" sId="1">
-    <oc r="W27" t="inlineStr">
-      <is>
-        <t>CURRENT SENCE CHIP RESISTOR 1W</t>
-      </is>
-    </oc>
-    <nc r="W27" t="inlineStr">
-      <is>
-        <t xml:space="preserve">CURRENT SENCE CHIP RESISTOR ±1% 1W </t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="14" sId="1">
-    <oc r="W28" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR</t>
-      </is>
-    </oc>
-    <nc r="W28" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR ±1% 1/16W</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="15" sId="1">
-    <oc r="W30" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR</t>
-      </is>
-    </oc>
-    <nc r="W30" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR ±1% 1/16W</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="16" sId="1">
-    <oc r="W31" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR</t>
-      </is>
-    </oc>
-    <nc r="W31" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR ±1% 1/16W</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="17" sId="1">
-    <oc r="W32" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR</t>
-      </is>
-    </oc>
-    <nc r="W32" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR ±1% 1/16W</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="18" sId="1">
-    <oc r="W33" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR</t>
-      </is>
-    </oc>
-    <nc r="W33" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR ±1% 1/16W</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="19" sId="1">
-    <oc r="W34" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR</t>
-      </is>
-    </oc>
-    <nc r="W34" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR ±1% 1/16W</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="20" sId="1">
-    <oc r="W35" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR</t>
-      </is>
-    </oc>
-    <nc r="W35" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR ±1% 1/16W</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="21" sId="1">
-    <oc r="W36" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR</t>
-      </is>
-    </oc>
-    <nc r="W36" t="inlineStr">
-      <is>
-        <t>CHIP RESISTOR ±1% 1/16W</t>
-      </is>
-    </nc>
-  </rcc>
-  <rrc rId="22" sId="1" ref="U1:U1048576" action="insertCol"/>
-  <rrc rId="23" sId="1" ref="U1:U1048576" action="insertCol"/>
-  <rcc rId="24" sId="1">
-    <nc r="U2">
-      <f>A2*50</f>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="U1:U1048576">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="25" sId="1">
-    <nc r="U3">
-      <f>A3*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="26" sId="1">
-    <nc r="U4">
-      <f>A4*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="27" sId="1">
-    <nc r="U5">
-      <f>A5*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="28" sId="1">
-    <nc r="U6">
-      <f>A6*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="29" sId="1">
-    <nc r="U7">
-      <f>A7*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="30" sId="1">
-    <nc r="U8">
-      <f>A8*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="31" sId="1">
-    <nc r="U9">
-      <f>A9*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="32" sId="1">
-    <nc r="U10">
-      <f>A10*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="33" sId="1">
-    <nc r="U11">
-      <f>A11*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="34" sId="1">
-    <nc r="U12">
-      <f>A12*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="35" sId="1">
-    <nc r="U13">
-      <f>A13*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="36" sId="1">
-    <nc r="U14">
-      <f>A14*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="37" sId="1">
-    <nc r="U15">
-      <f>A15*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="38" sId="1">
-    <nc r="U16">
-      <f>A16*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="39" sId="1">
-    <nc r="U17">
-      <f>A17*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="40" sId="1">
-    <nc r="U18">
-      <f>A18*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="41" sId="1">
-    <nc r="U19">
-      <f>A19*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="42" sId="1">
-    <nc r="U20">
-      <f>A20*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="43" sId="1">
-    <nc r="U21">
-      <f>A21*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="44" sId="1">
-    <nc r="U22">
-      <f>A22*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="45" sId="1">
-    <nc r="U23">
-      <f>A23*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="46" sId="1">
-    <nc r="U24">
-      <f>A24*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="47" sId="1">
-    <nc r="U25">
-      <f>A25*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="48" sId="1">
-    <nc r="U26">
-      <f>A26*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="49" sId="1">
-    <nc r="U27">
-      <f>A27*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="50" sId="1">
-    <nc r="U28">
-      <f>A28*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="51" sId="1">
-    <nc r="U29">
-      <f>A29*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="52" sId="1">
-    <nc r="U30">
-      <f>A30*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="53" sId="1">
-    <nc r="U31">
-      <f>A31*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="54" sId="1">
-    <nc r="U32">
-      <f>A32*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="55" sId="1">
-    <nc r="U33">
-      <f>A33*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="56" sId="1">
-    <nc r="U34">
-      <f>A34*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="57" sId="1">
-    <nc r="U35">
-      <f>A35*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="58" sId="1">
-    <nc r="U36">
-      <f>A36*50</f>
-    </nc>
-  </rcc>
-  <rcc rId="59" sId="1" numFmtId="11">
-    <nc r="K2">
-      <v>2.4287000000000001</v>
-    </nc>
-  </rcc>
-  <rcc rId="60" sId="1" numFmtId="11">
-    <nc r="M2">
-      <v>2.0653000000000001</v>
-    </nc>
-  </rcc>
-  <rcc rId="61" sId="1" numFmtId="11">
-    <nc r="N2">
-      <v>2.0653000000000001</v>
-    </nc>
-  </rcc>
-  <rcc rId="62" sId="1" numFmtId="11">
-    <nc r="O2">
-      <v>2.0653000000000001</v>
-    </nc>
-  </rcc>
-  <rcc rId="63" sId="1" numFmtId="11">
-    <nc r="P2">
-      <v>2.0653000000000001</v>
-    </nc>
-  </rcc>
-  <rcc rId="64" sId="1" numFmtId="11">
-    <nc r="Q2">
-      <v>2.0653000000000001</v>
-    </nc>
-  </rcc>
-  <rcc rId="65" sId="1" numFmtId="11">
-    <nc r="R2">
-      <v>2.0653000000000001</v>
-    </nc>
-  </rcc>
-  <rcc rId="66" sId="1">
-    <nc r="V2">
-      <f>IF(U2&lt;10,J2,IF(U2&lt;30,K2,IF(U2&lt;50,L2,IF(U2&lt;100,M2,IF(U2&lt;200,N2,IF(U2&lt;500,O2,IF(U2&lt;1000,P2,IF(U2&lt;2000,Q2,R2))))))))</f>
-    </nc>
-  </rcc>
-  <rcc rId="67" sId="1">
-    <nc r="U1" t="inlineStr">
-      <is>
-        <t>Pcs for 50 PCB</t>
-      </is>
-    </nc>
-  </rcc>
-  <rrc rId="68" sId="2" ref="C1:C1048576" action="insertCol"/>
-  <rcc rId="69" sId="2">
-    <nc r="C1" t="inlineStr">
-      <is>
-        <t>PRICE</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="70" sId="2">
-    <nc r="E1" t="inlineStr">
-      <is>
-        <t>PRICE_DATE</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="E1">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rrc rId="71" sId="2" ref="D1:D1048576" action="insertCol"/>
-  <rm rId="72" sheetId="2" source="F1:F1048576" destination="D1:D1048576" sourceSheetId="2">
-    <rfmt sheetId="2" xfDxf="1" sqref="D1:D1048576" start="0" length="0"/>
-    <rfmt sheetId="2" sqref="D1" start="0" length="0">
-      <dxf>
-        <font>
-          <b/>
-          <sz val="11"/>
-          <color theme="1"/>
-          <name val="Calibri"/>
-          <scheme val="minor"/>
-        </font>
-      </dxf>
-    </rfmt>
-  </rm>
-  <rrc rId="73" sId="2" ref="F1:F1048576" action="deleteCol">
-    <rfmt sheetId="2" xfDxf="1" sqref="F1:F1048576" start="0" length="0"/>
-  </rrc>
-  <rcc rId="74" sId="2">
-    <nc r="C2">
-      <v>0.55000000000000004</v>
-    </nc>
-  </rcc>
-  <rcc rId="75" sId="2" odxf="1" dxf="1" numFmtId="19">
-    <nc r="D2">
-      <v>43919</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="76" sId="2">
-    <nc r="F1" t="inlineStr">
-      <is>
-        <t>URL</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="F1">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="77" sId="2" xfDxf="1" dxf="1">
-    <nc r="F2" t="inlineStr">
-      <is>
-        <t>https://www.aliexpress.com/item/32821900056.html?spm=a2g0s.9042311.0.0.27424c4d7QpKiR</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="C1:C1048576">
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="78" sId="2" numFmtId="11">
-    <nc r="C3">
-      <v>4</v>
-    </nc>
-  </rcc>
-  <rcc rId="79" sId="2" odxf="1" dxf="1" numFmtId="19">
-    <nc r="D3">
-      <v>43919</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="80" sId="2" xfDxf="1" dxf="1">
-    <nc r="F3" t="inlineStr">
-      <is>
-        <t>https://www.aliexpress.com/item/33042530151.html?spm=a2g0o.detail.1000060.3.413116e3UwnGSp&amp;gps-id=pcDetailBottomMoreThisSeller&amp;scm=1007.14977.161855.0&amp;scm_id=1007.14977.161855.0&amp;scm-url=1007.14977.161855.0&amp;pvid=e7acc9bf-7b2c-452a-9ec7-bda6f01c289c&amp;_t=gps-id:pcDetailBottomMoreThisSeller,scm-url:1007.14977.161855.0,pvid:e7acc9bf-7b2c-452a-9ec7-bda6f01c289c,tpp_buckets:668%230%23165478%2314_668%23808%234093%23880_668%23888%233325%234</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="81" sId="1">
-    <nc r="V1" t="inlineStr">
-      <is>
-        <t>Price if 50 PCB</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>